<commit_message>
Added units into diagrams
</commit_message>
<xml_diff>
--- a/data/tech_conv_with_units.xlsx
+++ b/data/tech_conv_with_units.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuke\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CodeRepository\refue.ch-data-workspace\streamlit_apps\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A6C601-E757-4857-9F90-BBA76111EB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1F2A69-8555-4452-B4F2-47788C88012D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-11985" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="416">
   <si>
     <t>ehubX Tech ID</t>
   </si>
@@ -1228,13 +1228,70 @@
   </si>
   <si>
     <t>DAC</t>
+  </si>
+  <si>
+    <t>Input Ratios</t>
+  </si>
+  <si>
+    <t>Output Ratios</t>
+  </si>
+  <si>
+    <t>1, 0.051, 0.299</t>
+  </si>
+  <si>
+    <t>1, 0.09,0.231</t>
+  </si>
+  <si>
+    <t>1, 0.389</t>
+  </si>
+  <si>
+    <t>1.107, 0.284, 0.089</t>
+  </si>
+  <si>
+    <t>1, 0.584</t>
+  </si>
+  <si>
+    <t>0.7,0.085</t>
+  </si>
+  <si>
+    <t>1,0.656,0.17</t>
+  </si>
+  <si>
+    <t>1.168, 0.268</t>
+  </si>
+  <si>
+    <t>0.063, 0.7</t>
+  </si>
+  <si>
+    <t>1,0.55</t>
+  </si>
+  <si>
+    <t>1.234, 0.316, 0.126</t>
+  </si>
+  <si>
+    <t>1, 0.561</t>
+  </si>
+  <si>
+    <t>0.55, 0.085</t>
+  </si>
+  <si>
+    <t>1, 0.139</t>
+  </si>
+  <si>
+    <t>0.879, 0.127</t>
+  </si>
+  <si>
+    <t>1, 0.271</t>
+  </si>
+  <si>
+    <t>0.158, 0.305, 0.993</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1249,6 +1306,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1286,9 +1348,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1595,13 +1660,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G175"/>
+  <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C134" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B46" sqref="B46"/>
+      <selection pane="bottomRight" activeCell="G159" sqref="G159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1613,9 +1678,11 @@
     <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1637,8 +1704,14 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1660,8 +1733,14 @@
       <c r="G2" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>322</v>
+      </c>
+      <c r="I2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1683,8 +1762,14 @@
       <c r="G3" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>322</v>
+      </c>
+      <c r="I3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1706,8 +1791,14 @@
       <c r="G4" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>322</v>
+      </c>
+      <c r="I4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1729,8 +1820,14 @@
       <c r="G5" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>322</v>
+      </c>
+      <c r="I5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1752,8 +1849,14 @@
       <c r="G6" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>322</v>
+      </c>
+      <c r="I6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1775,8 +1878,14 @@
       <c r="G7" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>322</v>
+      </c>
+      <c r="I7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1798,8 +1907,14 @@
       <c r="G8" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>322</v>
+      </c>
+      <c r="I8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1821,8 +1936,14 @@
       <c r="G9" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>322</v>
+      </c>
+      <c r="I9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1844,8 +1965,14 @@
       <c r="G10" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>322</v>
+      </c>
+      <c r="I10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1867,8 +1994,14 @@
       <c r="G11" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>322</v>
+      </c>
+      <c r="I11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1890,8 +2023,14 @@
       <c r="G12" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>322</v>
+      </c>
+      <c r="I12" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1913,8 +2052,14 @@
       <c r="G13" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>322</v>
+      </c>
+      <c r="I13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1936,8 +2081,14 @@
       <c r="G14" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>322</v>
+      </c>
+      <c r="I14" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1959,8 +2110,14 @@
       <c r="G15" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>322</v>
+      </c>
+      <c r="I15" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1982,8 +2139,14 @@
       <c r="G16" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>322</v>
+      </c>
+      <c r="I16" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2005,8 +2168,14 @@
       <c r="G17" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17" t="s">
+        <v>322</v>
+      </c>
+      <c r="I17" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2028,8 +2197,14 @@
       <c r="G18" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>322</v>
+      </c>
+      <c r="I18" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2051,8 +2226,14 @@
       <c r="G19" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19" t="s">
+        <v>322</v>
+      </c>
+      <c r="I19" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2074,8 +2255,14 @@
       <c r="G20" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>322</v>
+      </c>
+      <c r="I20" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2097,8 +2284,14 @@
       <c r="G21" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
+        <v>322</v>
+      </c>
+      <c r="I21" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2120,8 +2313,14 @@
       <c r="G22" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
+        <v>322</v>
+      </c>
+      <c r="I22" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -2143,8 +2342,14 @@
       <c r="G23" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23" t="s">
+        <v>322</v>
+      </c>
+      <c r="I23" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2166,8 +2371,14 @@
       <c r="G24" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>322</v>
+      </c>
+      <c r="I24" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2189,8 +2400,14 @@
       <c r="G25" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>322</v>
+      </c>
+      <c r="I25" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2212,8 +2429,14 @@
       <c r="G26" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>322</v>
+      </c>
+      <c r="I26" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -2235,8 +2458,14 @@
       <c r="G27" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27" t="s">
+        <v>322</v>
+      </c>
+      <c r="I27" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -2258,8 +2487,14 @@
       <c r="G28" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H28" t="s">
+        <v>322</v>
+      </c>
+      <c r="I28" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -2281,8 +2516,14 @@
       <c r="G29" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29" t="s">
+        <v>322</v>
+      </c>
+      <c r="I29" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -2304,8 +2545,14 @@
       <c r="G30" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>322</v>
+      </c>
+      <c r="I30" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -2327,8 +2574,14 @@
       <c r="G31" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31" t="s">
+        <v>322</v>
+      </c>
+      <c r="I31" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2350,8 +2603,14 @@
       <c r="G32" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
+        <v>322</v>
+      </c>
+      <c r="I32" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -2373,8 +2632,14 @@
       <c r="G33" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>322</v>
+      </c>
+      <c r="I33" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -2396,8 +2661,14 @@
       <c r="G34" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>322</v>
+      </c>
+      <c r="I34" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -2419,8 +2690,14 @@
       <c r="G35" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>322</v>
+      </c>
+      <c r="I35" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2442,8 +2719,14 @@
       <c r="G36" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H36" t="s">
+        <v>322</v>
+      </c>
+      <c r="I36" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2465,8 +2748,14 @@
       <c r="G37" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H37" t="s">
+        <v>322</v>
+      </c>
+      <c r="I37" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -2488,8 +2777,14 @@
       <c r="G38" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38" t="s">
+        <v>322</v>
+      </c>
+      <c r="I38" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -2511,8 +2806,14 @@
       <c r="G39" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H39" t="s">
+        <v>322</v>
+      </c>
+      <c r="I39" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2534,8 +2835,14 @@
       <c r="G40" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H40" t="s">
+        <v>322</v>
+      </c>
+      <c r="I40" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -2557,8 +2864,14 @@
       <c r="G41" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H41" t="s">
+        <v>322</v>
+      </c>
+      <c r="I41" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -2580,8 +2893,14 @@
       <c r="G42" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H42" t="s">
+        <v>322</v>
+      </c>
+      <c r="I42" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2603,8 +2922,14 @@
       <c r="G43" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H43" t="s">
+        <v>322</v>
+      </c>
+      <c r="I43" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -2626,8 +2951,14 @@
       <c r="G44" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H44" t="s">
+        <v>322</v>
+      </c>
+      <c r="I44" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2649,8 +2980,14 @@
       <c r="G45" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H45" t="s">
+        <v>322</v>
+      </c>
+      <c r="I45" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2672,8 +3009,14 @@
       <c r="G46" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H46" t="s">
+        <v>322</v>
+      </c>
+      <c r="I46" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -2695,8 +3038,14 @@
       <c r="G47" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H47" t="s">
+        <v>322</v>
+      </c>
+      <c r="I47" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2718,8 +3067,14 @@
       <c r="G48" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H48" t="s">
+        <v>322</v>
+      </c>
+      <c r="I48" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -2741,8 +3096,14 @@
       <c r="G49" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H49" t="s">
+        <v>322</v>
+      </c>
+      <c r="I49" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -2764,8 +3125,14 @@
       <c r="G50" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H50" t="s">
+        <v>322</v>
+      </c>
+      <c r="I50" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -2787,8 +3154,14 @@
       <c r="G51" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H51" t="s">
+        <v>322</v>
+      </c>
+      <c r="I51" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -2810,8 +3183,14 @@
       <c r="G52" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H52" t="s">
+        <v>322</v>
+      </c>
+      <c r="I52" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -2833,8 +3212,14 @@
       <c r="G53" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H53" t="s">
+        <v>322</v>
+      </c>
+      <c r="I53" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -2856,8 +3241,14 @@
       <c r="G54" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H54" t="s">
+        <v>322</v>
+      </c>
+      <c r="I54" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -2879,8 +3270,14 @@
       <c r="G55" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H55" t="s">
+        <v>322</v>
+      </c>
+      <c r="I55" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -2902,8 +3299,14 @@
       <c r="G56" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H56" t="s">
+        <v>322</v>
+      </c>
+      <c r="I56" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -2925,8 +3328,14 @@
       <c r="G57" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H57" t="s">
+        <v>322</v>
+      </c>
+      <c r="I57" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -2948,8 +3357,14 @@
       <c r="G58" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H58" t="s">
+        <v>322</v>
+      </c>
+      <c r="I58" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -2971,8 +3386,14 @@
       <c r="G59" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H59" t="s">
+        <v>322</v>
+      </c>
+      <c r="I59" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -2994,8 +3415,14 @@
       <c r="G60" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H60" t="s">
+        <v>322</v>
+      </c>
+      <c r="I60" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -3017,8 +3444,14 @@
       <c r="G61" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H61" t="s">
+        <v>322</v>
+      </c>
+      <c r="I61" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -3040,8 +3473,14 @@
       <c r="G62" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H62" t="s">
+        <v>322</v>
+      </c>
+      <c r="I62" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -3063,8 +3502,14 @@
       <c r="G63" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H63" t="s">
+        <v>322</v>
+      </c>
+      <c r="I63" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -3086,8 +3531,14 @@
       <c r="G64" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H64" t="s">
+        <v>322</v>
+      </c>
+      <c r="I64" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -3109,8 +3560,14 @@
       <c r="G65" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H65" t="s">
+        <v>322</v>
+      </c>
+      <c r="I65" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -3132,8 +3589,14 @@
       <c r="G66" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H66" t="s">
+        <v>322</v>
+      </c>
+      <c r="I66" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -3155,8 +3618,14 @@
       <c r="G67" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H67" t="s">
+        <v>322</v>
+      </c>
+      <c r="I67" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -3178,8 +3647,14 @@
       <c r="G68" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H68" t="s">
+        <v>322</v>
+      </c>
+      <c r="I68" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -3201,8 +3676,14 @@
       <c r="G69" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H69" t="s">
+        <v>322</v>
+      </c>
+      <c r="I69" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -3224,8 +3705,14 @@
       <c r="G70" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H70" t="s">
+        <v>322</v>
+      </c>
+      <c r="I70" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -3247,8 +3734,14 @@
       <c r="G71" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H71" t="s">
+        <v>322</v>
+      </c>
+      <c r="I71" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -3270,8 +3763,14 @@
       <c r="G72" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H72" t="s">
+        <v>322</v>
+      </c>
+      <c r="I72" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -3293,8 +3792,14 @@
       <c r="G73" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H73" t="s">
+        <v>322</v>
+      </c>
+      <c r="I73" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -3316,8 +3821,14 @@
       <c r="G74" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H74" t="s">
+        <v>322</v>
+      </c>
+      <c r="I74" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>77</v>
       </c>
@@ -3339,8 +3850,14 @@
       <c r="G75" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H75" t="s">
+        <v>322</v>
+      </c>
+      <c r="I75" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>78</v>
       </c>
@@ -3362,8 +3879,14 @@
       <c r="G76" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H76" t="s">
+        <v>322</v>
+      </c>
+      <c r="I76" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -3385,8 +3908,14 @@
       <c r="G77" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H77" t="s">
+        <v>322</v>
+      </c>
+      <c r="I77" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -3408,8 +3937,14 @@
       <c r="G78" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H78" t="s">
+        <v>322</v>
+      </c>
+      <c r="I78" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -3431,8 +3966,14 @@
       <c r="G79" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H79" t="s">
+        <v>322</v>
+      </c>
+      <c r="I79" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -3454,8 +3995,14 @@
       <c r="G80" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H80" t="s">
+        <v>322</v>
+      </c>
+      <c r="I80" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>83</v>
       </c>
@@ -3477,8 +4024,14 @@
       <c r="G81" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H81" t="s">
+        <v>322</v>
+      </c>
+      <c r="I81" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>84</v>
       </c>
@@ -3500,8 +4053,14 @@
       <c r="G82" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H82" t="s">
+        <v>322</v>
+      </c>
+      <c r="I82" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>85</v>
       </c>
@@ -3523,8 +4082,14 @@
       <c r="G83" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H83" t="s">
+        <v>322</v>
+      </c>
+      <c r="I83" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>86</v>
       </c>
@@ -3546,8 +4111,14 @@
       <c r="G84" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H84" t="s">
+        <v>322</v>
+      </c>
+      <c r="I84" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -3569,8 +4140,14 @@
       <c r="G85" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H85" t="s">
+        <v>322</v>
+      </c>
+      <c r="I85" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>88</v>
       </c>
@@ -3592,8 +4169,14 @@
       <c r="G86" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H86" t="s">
+        <v>322</v>
+      </c>
+      <c r="I86" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>89</v>
       </c>
@@ -3615,8 +4198,14 @@
       <c r="G87" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H87" t="s">
+        <v>322</v>
+      </c>
+      <c r="I87" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>90</v>
       </c>
@@ -3638,8 +4227,14 @@
       <c r="G88" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H88" t="s">
+        <v>322</v>
+      </c>
+      <c r="I88" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>91</v>
       </c>
@@ -3661,8 +4256,14 @@
       <c r="G89" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H89" t="s">
+        <v>322</v>
+      </c>
+      <c r="I89" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>92</v>
       </c>
@@ -3684,8 +4285,14 @@
       <c r="G90" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H90" t="s">
+        <v>322</v>
+      </c>
+      <c r="I90" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>93</v>
       </c>
@@ -3707,8 +4314,11 @@
       <c r="G91" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H91" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>94</v>
       </c>
@@ -3730,8 +4340,14 @@
       <c r="G92" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H92" t="s">
+        <v>400</v>
+      </c>
+      <c r="I92">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>95</v>
       </c>
@@ -3753,8 +4369,11 @@
       <c r="G93" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H93" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>96</v>
       </c>
@@ -3776,8 +4395,14 @@
       <c r="G94" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H94" t="s">
+        <v>400</v>
+      </c>
+      <c r="I94">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>97</v>
       </c>
@@ -3799,8 +4424,14 @@
       <c r="G95" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H95" t="s">
+        <v>322</v>
+      </c>
+      <c r="I95" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>98</v>
       </c>
@@ -3822,8 +4453,14 @@
       <c r="G96" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H96" t="s">
+        <v>322</v>
+      </c>
+      <c r="I96" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -3845,8 +4482,14 @@
       <c r="G97" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H97" t="s">
+        <v>322</v>
+      </c>
+      <c r="I97" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>100</v>
       </c>
@@ -3868,8 +4511,14 @@
       <c r="G98" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H98" t="s">
+        <v>322</v>
+      </c>
+      <c r="I98" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -3891,8 +4540,14 @@
       <c r="G99" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H99" t="s">
+        <v>322</v>
+      </c>
+      <c r="I99" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -3914,8 +4569,14 @@
       <c r="G100" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H100" t="s">
+        <v>322</v>
+      </c>
+      <c r="I100" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>103</v>
       </c>
@@ -3937,8 +4598,14 @@
       <c r="G101" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H101" t="s">
+        <v>322</v>
+      </c>
+      <c r="I101" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>104</v>
       </c>
@@ -3960,8 +4627,14 @@
       <c r="G102" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H102" t="s">
+        <v>322</v>
+      </c>
+      <c r="I102" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>105</v>
       </c>
@@ -3983,8 +4656,14 @@
       <c r="G103" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H103" t="s">
+        <v>322</v>
+      </c>
+      <c r="I103" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>106</v>
       </c>
@@ -4006,8 +4685,14 @@
       <c r="G104" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H104" t="s">
+        <v>322</v>
+      </c>
+      <c r="I104" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -4029,8 +4714,14 @@
       <c r="G105" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H105" t="s">
+        <v>322</v>
+      </c>
+      <c r="I105" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>108</v>
       </c>
@@ -4052,8 +4743,14 @@
       <c r="G106" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H106" t="s">
+        <v>322</v>
+      </c>
+      <c r="I106" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>109</v>
       </c>
@@ -4075,8 +4772,14 @@
       <c r="G107" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H107" t="s">
+        <v>322</v>
+      </c>
+      <c r="I107" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>110</v>
       </c>
@@ -4098,8 +4801,14 @@
       <c r="G108" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H108" t="s">
+        <v>322</v>
+      </c>
+      <c r="I108" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>111</v>
       </c>
@@ -4121,8 +4830,14 @@
       <c r="G109" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H109" t="s">
+        <v>322</v>
+      </c>
+      <c r="I109" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>112</v>
       </c>
@@ -4144,8 +4859,14 @@
       <c r="G110" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H110" t="s">
+        <v>322</v>
+      </c>
+      <c r="I110" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>113</v>
       </c>
@@ -4167,8 +4888,14 @@
       <c r="G111" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H111" t="s">
+        <v>322</v>
+      </c>
+      <c r="I111" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>114</v>
       </c>
@@ -4190,8 +4917,14 @@
       <c r="G112" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H112" t="s">
+        <v>322</v>
+      </c>
+      <c r="I112" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>115</v>
       </c>
@@ -4213,8 +4946,14 @@
       <c r="G113" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H113" t="s">
+        <v>322</v>
+      </c>
+      <c r="I113" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>116</v>
       </c>
@@ -4236,8 +4975,14 @@
       <c r="G114" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H114" t="s">
+        <v>322</v>
+      </c>
+      <c r="I114" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>117</v>
       </c>
@@ -4259,8 +5004,14 @@
       <c r="G115" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H115" t="s">
+        <v>322</v>
+      </c>
+      <c r="I115" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>118</v>
       </c>
@@ -4282,8 +5033,14 @@
       <c r="G116" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H116" t="s">
+        <v>322</v>
+      </c>
+      <c r="I116" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>119</v>
       </c>
@@ -4305,8 +5062,14 @@
       <c r="G117" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H117" t="s">
+        <v>322</v>
+      </c>
+      <c r="I117" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>120</v>
       </c>
@@ -4328,8 +5091,14 @@
       <c r="G118" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H118" t="s">
+        <v>322</v>
+      </c>
+      <c r="I118" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>121</v>
       </c>
@@ -4351,8 +5120,14 @@
       <c r="G119" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H119" t="s">
+        <v>322</v>
+      </c>
+      <c r="I119" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>122</v>
       </c>
@@ -4374,8 +5149,14 @@
       <c r="G120" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H120" t="s">
+        <v>322</v>
+      </c>
+      <c r="I120" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>123</v>
       </c>
@@ -4397,8 +5178,14 @@
       <c r="G121" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H121" t="s">
+        <v>322</v>
+      </c>
+      <c r="I121" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>124</v>
       </c>
@@ -4420,8 +5207,14 @@
       <c r="G122" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H122" t="s">
+        <v>322</v>
+      </c>
+      <c r="I122" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>125</v>
       </c>
@@ -4443,8 +5236,14 @@
       <c r="G123" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H123" t="s">
+        <v>322</v>
+      </c>
+      <c r="I123" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>126</v>
       </c>
@@ -4466,8 +5265,14 @@
       <c r="G124" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H124" t="s">
+        <v>322</v>
+      </c>
+      <c r="I124" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>127</v>
       </c>
@@ -4489,8 +5294,14 @@
       <c r="G125" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H125" t="s">
+        <v>322</v>
+      </c>
+      <c r="I125" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>128</v>
       </c>
@@ -4512,8 +5323,14 @@
       <c r="G126" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H126" t="s">
+        <v>322</v>
+      </c>
+      <c r="I126" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>129</v>
       </c>
@@ -4535,8 +5352,14 @@
       <c r="G127" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H127" t="s">
+        <v>322</v>
+      </c>
+      <c r="I127" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>130</v>
       </c>
@@ -4558,8 +5381,14 @@
       <c r="G128" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H128" t="s">
+        <v>322</v>
+      </c>
+      <c r="I128" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>131</v>
       </c>
@@ -4581,8 +5410,14 @@
       <c r="G129" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H129" t="s">
+        <v>322</v>
+      </c>
+      <c r="I129" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>132</v>
       </c>
@@ -4604,8 +5439,14 @@
       <c r="G130" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H130" t="s">
+        <v>322</v>
+      </c>
+      <c r="I130" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>133</v>
       </c>
@@ -4627,8 +5468,14 @@
       <c r="G131" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H131" t="s">
+        <v>401</v>
+      </c>
+      <c r="I131" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>134</v>
       </c>
@@ -4650,8 +5497,14 @@
       <c r="G132" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H132" t="s">
+        <v>401</v>
+      </c>
+      <c r="I132" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>135</v>
       </c>
@@ -4673,8 +5526,14 @@
       <c r="G133" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H133" t="s">
+        <v>401</v>
+      </c>
+      <c r="I133" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>136</v>
       </c>
@@ -4696,8 +5555,14 @@
       <c r="G134" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H134" t="s">
+        <v>401</v>
+      </c>
+      <c r="I134" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>137</v>
       </c>
@@ -4719,8 +5584,14 @@
       <c r="G135" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H135" t="s">
+        <v>401</v>
+      </c>
+      <c r="I135" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>138</v>
       </c>
@@ -4742,8 +5613,14 @@
       <c r="G136" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H136" t="s">
+        <v>401</v>
+      </c>
+      <c r="I136" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>139</v>
       </c>
@@ -4765,8 +5642,14 @@
       <c r="G137" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H137" t="s">
+        <v>401</v>
+      </c>
+      <c r="I137" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>140</v>
       </c>
@@ -4788,8 +5671,14 @@
       <c r="G138" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H138" t="s">
+        <v>403</v>
+      </c>
+      <c r="I138" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>141</v>
       </c>
@@ -4811,8 +5700,14 @@
       <c r="G139" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H139" t="s">
+        <v>403</v>
+      </c>
+      <c r="I139" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>142</v>
       </c>
@@ -4834,8 +5729,14 @@
       <c r="G140" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H140" t="s">
+        <v>403</v>
+      </c>
+      <c r="I140" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>143</v>
       </c>
@@ -4857,8 +5758,14 @@
       <c r="G141" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H141" t="s">
+        <v>403</v>
+      </c>
+      <c r="I141" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>144</v>
       </c>
@@ -4880,8 +5787,14 @@
       <c r="G142" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H142" t="s">
+        <v>403</v>
+      </c>
+      <c r="I142" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>145</v>
       </c>
@@ -4903,8 +5816,14 @@
       <c r="G143" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H143" t="s">
+        <v>403</v>
+      </c>
+      <c r="I143" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>146</v>
       </c>
@@ -4926,8 +5845,14 @@
       <c r="G144" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H144" t="s">
+        <v>322</v>
+      </c>
+      <c r="I144" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>147</v>
       </c>
@@ -4949,8 +5874,14 @@
       <c r="G145" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H145" t="s">
+        <v>322</v>
+      </c>
+      <c r="I145" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>148</v>
       </c>
@@ -4972,8 +5903,14 @@
       <c r="G146" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H146" t="s">
+        <v>322</v>
+      </c>
+      <c r="I146" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>149</v>
       </c>
@@ -4995,8 +5932,14 @@
       <c r="G147" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H147" t="s">
+        <v>322</v>
+      </c>
+      <c r="I147" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>150</v>
       </c>
@@ -5018,8 +5961,14 @@
       <c r="G148" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H148" t="s">
+        <v>322</v>
+      </c>
+      <c r="I148" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>151</v>
       </c>
@@ -5041,8 +5990,14 @@
       <c r="G149" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H149" t="s">
+        <v>322</v>
+      </c>
+      <c r="I149" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>152</v>
       </c>
@@ -5064,8 +6019,14 @@
       <c r="G150" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H150" t="s">
+        <v>322</v>
+      </c>
+      <c r="I150" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>153</v>
       </c>
@@ -5087,8 +6048,14 @@
       <c r="G151" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H151" t="s">
+        <v>322</v>
+      </c>
+      <c r="I151" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>154</v>
       </c>
@@ -5110,8 +6077,14 @@
       <c r="G152" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H152" t="s">
+        <v>322</v>
+      </c>
+      <c r="I152" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>155</v>
       </c>
@@ -5133,8 +6106,14 @@
       <c r="G153" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H153" t="s">
+        <v>322</v>
+      </c>
+      <c r="I153" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>156</v>
       </c>
@@ -5156,8 +6135,14 @@
       <c r="G154" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H154" t="s">
+        <v>322</v>
+      </c>
+      <c r="I154" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>157</v>
       </c>
@@ -5179,8 +6164,14 @@
       <c r="G155" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H155" t="s">
+        <v>322</v>
+      </c>
+      <c r="I155" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>158</v>
       </c>
@@ -5202,8 +6193,14 @@
       <c r="G156" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H156" t="s">
+        <v>322</v>
+      </c>
+      <c r="I156" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>159</v>
       </c>
@@ -5223,10 +6220,16 @@
         <v>343</v>
       </c>
       <c r="G157" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+      <c r="H157" t="s">
+        <v>405</v>
+      </c>
+      <c r="I157" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>160</v>
       </c>
@@ -5246,10 +6249,16 @@
         <v>343</v>
       </c>
       <c r="G158" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+      <c r="H158" t="s">
+        <v>405</v>
+      </c>
+      <c r="I158" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>161</v>
       </c>
@@ -5271,8 +6280,14 @@
       <c r="G159" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H159" t="s">
+        <v>322</v>
+      </c>
+      <c r="I159" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>162</v>
       </c>
@@ -5294,8 +6309,14 @@
       <c r="G160" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H160" t="s">
+        <v>322</v>
+      </c>
+      <c r="I160" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>163</v>
       </c>
@@ -5317,8 +6338,14 @@
       <c r="G161" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H161" t="s">
+        <v>322</v>
+      </c>
+      <c r="I161" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>164</v>
       </c>
@@ -5340,8 +6367,14 @@
       <c r="G162" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H162" t="s">
+        <v>322</v>
+      </c>
+      <c r="I162" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>165</v>
       </c>
@@ -5363,8 +6396,14 @@
       <c r="G163" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H163" t="s">
+        <v>322</v>
+      </c>
+      <c r="I163" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>166</v>
       </c>
@@ -5386,8 +6425,14 @@
       <c r="G164" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H164" t="s">
+        <v>408</v>
+      </c>
+      <c r="I164" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>167</v>
       </c>
@@ -5409,8 +6454,14 @@
       <c r="G165" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H165" t="s">
+        <v>408</v>
+      </c>
+      <c r="I165" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>168</v>
       </c>
@@ -5432,8 +6483,14 @@
       <c r="G166" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H166" t="s">
+        <v>408</v>
+      </c>
+      <c r="I166" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>169</v>
       </c>
@@ -5455,8 +6512,14 @@
       <c r="G167" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H167" t="s">
+        <v>408</v>
+      </c>
+      <c r="I167" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>170</v>
       </c>
@@ -5478,8 +6541,14 @@
       <c r="G168" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H168" t="s">
+        <v>410</v>
+      </c>
+      <c r="I168" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>171</v>
       </c>
@@ -5501,8 +6570,14 @@
       <c r="G169" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H169" t="s">
+        <v>322</v>
+      </c>
+      <c r="I169" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>172</v>
       </c>
@@ -5524,8 +6599,14 @@
       <c r="G170" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H170" t="s">
+        <v>322</v>
+      </c>
+      <c r="I170" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>173</v>
       </c>
@@ -5547,8 +6628,14 @@
       <c r="G171" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H171" t="s">
+        <v>322</v>
+      </c>
+      <c r="I171" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>174</v>
       </c>
@@ -5570,8 +6657,14 @@
       <c r="G172" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H172" t="s">
+        <v>322</v>
+      </c>
+      <c r="I172" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>175</v>
       </c>
@@ -5593,8 +6686,14 @@
       <c r="G173" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H173" t="s">
+        <v>412</v>
+      </c>
+      <c r="I173" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>176</v>
       </c>
@@ -5613,8 +6712,14 @@
       <c r="G174" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H174" t="s">
+        <v>414</v>
+      </c>
+      <c r="I174" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>177</v>
       </c>
@@ -5632,6 +6737,12 @@
       </c>
       <c r="G175" t="s">
         <v>355</v>
+      </c>
+      <c r="H175" t="s">
+        <v>414</v>
+      </c>
+      <c r="I175" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>